<commit_message>
Updated SO LUI TC upto Invoice creation
</commit_message>
<xml_diff>
--- a/templates/DEVQAFF/SalesOrder_LUI.xlsx
+++ b/templates/DEVQAFF/SalesOrder_LUI.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_AutomationOrg\rsqasampleproj\templates\DEVQAFF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\DEVQAFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BF442A0-4021-4473-A245-9840855421E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4F12A5-7956-4CD0-975F-6132421D8305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Customer</t>
   </si>
@@ -53,6 +53,9 @@
   </si>
   <si>
     <t>Conf_prod-No_track (purType)</t>
+  </si>
+  <si>
+    <t>ProductTypeIndex</t>
   </si>
 </sst>
 </file>
@@ -404,38 +407,48 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A018314-DE04-4A79-AD08-915EB1DA286B}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated SO LUI TC with workaround for SOINV page opening issue
</commit_message>
<xml_diff>
--- a/templates/DEVQAFF/SalesOrder_LUI.xlsx
+++ b/templates/DEVQAFF/SalesOrder_LUI.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ashok\Provar\RSTK_Automation\rsqasampleproj\templates\DEVQAFF\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF4F12A5-7956-4CD0-975F-6132421D8305}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3C366E0-C08E-4847-9C99-493D9F2103A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddHeader" sheetId="1" r:id="rId1"/>
     <sheet name="AddLine" sheetId="2" r:id="rId2"/>
+    <sheet name="Invoice" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Customer</t>
   </si>
@@ -56,6 +57,12 @@
   </si>
   <si>
     <t>ProductTypeIndex</t>
+  </si>
+  <si>
+    <t>InvoicePage_URL</t>
+  </si>
+  <si>
+    <t>https://rstk-dev-qa-ff.lightning.force.com/lightning/r/rstk__soinv__c/</t>
   </si>
 </sst>
 </file>
@@ -409,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A018314-DE04-4A79-AD08-915EB1DA286B}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -456,4 +463,32 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41AC6277-F927-4837-84C0-1EA27C4A85F9}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>